<commit_message>
Relatório de testes alterado
</commit_message>
<xml_diff>
--- a/Relatório de teste.xlsx
+++ b/Relatório de teste.xlsx
@@ -958,7 +958,7 @@
         </is>
       </c>
       <c r="C16" s="9" t="n">
-        <v>44796.60637254047</v>
+        <v>44796.64952684756</v>
       </c>
       <c r="D16" s="12" t="inlineStr">
         <is>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="C18" s="9" t="n">
-        <v>44796.60637254047</v>
+        <v>44796.64952684756</v>
       </c>
       <c r="D18" s="12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Adicionado funcionalidade de escolher um dos seis testes do CompararSaidaBasico. Adicionado funcionalidade de definir o delimitador do arquivo sas. Alterado template, eliminando as figuras
</commit_message>
<xml_diff>
--- a/Relatório de teste.xlsx
+++ b/Relatório de teste.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6210" yWindow="1050" windowWidth="13470" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -89,7 +89,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -98,6 +98,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -118,6 +129,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="hair">
@@ -155,27 +179,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="hair">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -202,9 +226,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -225,105 +252,52 @@
     <xf numFmtId="164" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <colors/>
 </styleSheet>
 </file>
 
@@ -630,18 +604,18 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="3" customWidth="1" style="14" min="1" max="1"/>
-    <col width="30.5703125" bestFit="1" customWidth="1" style="14" min="2" max="2"/>
-    <col width="20.42578125" customWidth="1" style="14" min="3" max="3"/>
-    <col width="23.42578125" customWidth="1" style="14" min="4" max="4"/>
-    <col width="27" customWidth="1" style="14" min="5" max="5"/>
-    <col width="27.140625" customWidth="1" style="14" min="6" max="6"/>
+    <col width="3" customWidth="1" min="1" max="1"/>
+    <col width="30.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="20.42578125" customWidth="1" min="3" max="3"/>
+    <col width="23.42578125" customWidth="1" min="4" max="4"/>
+    <col width="27" customWidth="1" min="5" max="5"/>
+    <col width="27.140625" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -656,59 +630,59 @@
       <c r="G2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="15" t="inlineStr">
+      <c r="A3" s="14" t="inlineStr">
         <is>
           <t>Arquivo original</t>
         </is>
       </c>
-      <c r="C3" s="19" t="inlineStr">
+      <c r="C3" s="21" t="inlineStr">
         <is>
           <t>exported_data_sas.csv</t>
         </is>
       </c>
-      <c r="D3" s="20" t="n"/>
-      <c r="E3" s="20" t="n"/>
-      <c r="F3" s="21" t="n"/>
+      <c r="D3" s="22" t="n"/>
+      <c r="E3" s="22" t="n"/>
+      <c r="F3" s="23" t="n"/>
       <c r="G3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="15" t="inlineStr">
+      <c r="A4" s="14" t="inlineStr">
         <is>
           <t>Arquivo convertido</t>
         </is>
       </c>
-      <c r="C4" s="16" t="inlineStr">
+      <c r="C4" s="24" t="inlineStr">
         <is>
           <t>exported_data_databricks.csv</t>
         </is>
       </c>
-      <c r="D4" s="17" t="n"/>
-      <c r="E4" s="17" t="n"/>
-      <c r="F4" s="18" t="n"/>
+      <c r="D4" s="25" t="n"/>
+      <c r="E4" s="25" t="n"/>
+      <c r="F4" s="26" t="n"/>
       <c r="G4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="inlineStr">
+      <c r="A5" s="14" t="inlineStr">
         <is>
           <t>Script avaliado</t>
         </is>
       </c>
-      <c r="C5" s="16" t="n"/>
-      <c r="D5" s="17" t="n"/>
-      <c r="E5" s="17" t="n"/>
-      <c r="F5" s="18" t="n"/>
+      <c r="C5" s="24" t="n"/>
+      <c r="D5" s="25" t="n"/>
+      <c r="E5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
       <c r="G5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="15" t="inlineStr">
+      <c r="A6" s="14" t="inlineStr">
         <is>
           <t>Tester</t>
         </is>
       </c>
-      <c r="C6" s="16" t="n"/>
-      <c r="D6" s="17" t="n"/>
-      <c r="E6" s="17" t="n"/>
-      <c r="F6" s="18" t="n"/>
+      <c r="C6" s="24" t="n"/>
+      <c r="D6" s="25" t="n"/>
+      <c r="E6" s="25" t="n"/>
+      <c r="F6" s="26" t="n"/>
       <c r="G6" s="1" t="n"/>
     </row>
     <row r="7">
@@ -721,32 +695,32 @@
       <c r="G7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="inlineStr">
+      <c r="A8" s="14" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B8" s="15" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <is>
           <t>caso de teste</t>
         </is>
       </c>
-      <c r="C8" s="15" t="inlineStr">
+      <c r="C8" s="14" t="inlineStr">
         <is>
           <t>data de execução</t>
         </is>
       </c>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="D8" s="14" t="inlineStr">
         <is>
           <t>relatório sas</t>
         </is>
       </c>
-      <c r="E8" s="15" t="inlineStr">
+      <c r="E8" s="14" t="inlineStr">
         <is>
           <t>relatório databricks</t>
         </is>
       </c>
-      <c r="F8" s="15" t="inlineStr">
+      <c r="F8" s="14" t="inlineStr">
         <is>
           <t>resultado final</t>
         </is>
@@ -754,16 +728,16 @@
       <c r="G8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>Formato dos Arquivos</t>
         </is>
       </c>
-      <c r="C9" s="8" t="n">
-        <v>44796.60558695602</v>
+      <c r="C9" s="9" t="n">
+        <v>44799.63413562386</v>
       </c>
       <c r="D9" s="11" t="inlineStr">
         <is>
@@ -775,7 +749,7 @@
           <t>.csv</t>
         </is>
       </c>
-      <c r="F9" s="7" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>APROVADO</t>
         </is>
@@ -783,16 +757,16 @@
       <c r="G9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>Quantidade de linhas</t>
         </is>
       </c>
-      <c r="C10" s="9" t="n">
-        <v>44796.60558695602</v>
+      <c r="C10" s="10" t="n">
+        <v>44799.63413567019</v>
       </c>
       <c r="D10" s="12" t="n">
         <v>8</v>
@@ -800,7 +774,7 @@
       <c r="E10" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="F10" s="6" t="inlineStr">
+      <c r="F10" s="7" t="inlineStr">
         <is>
           <t>APROVADO</t>
         </is>
@@ -808,16 +782,16 @@
       <c r="G10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>Quantidade de colunas</t>
         </is>
       </c>
-      <c r="C11" s="8" t="n">
-        <v>44796.60558695602</v>
+      <c r="C11" s="9" t="n">
+        <v>44799.6341357049</v>
       </c>
       <c r="D11" s="11" t="n">
         <v>5</v>
@@ -825,24 +799,24 @@
       <c r="E11" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F11" s="7" t="inlineStr">
+      <c r="F11" s="8" t="inlineStr">
         <is>
           <t>APROVADO</t>
         </is>
       </c>
       <c r="G11" s="1" t="n"/>
     </row>
-    <row r="12" ht="30" customHeight="1" s="14">
-      <c r="A12" s="5" t="n">
+    <row r="12">
+      <c r="A12" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" s="4" t="inlineStr">
         <is>
           <t>Conteúdo das colunas</t>
         </is>
       </c>
-      <c r="C12" s="9" t="n">
-        <v>44796.60558695602</v>
+      <c r="C12" s="10" t="n">
+        <v>44799.63413572805</v>
       </c>
       <c r="D12" s="12" t="inlineStr">
         <is>
@@ -854,171 +828,129 @@
           <t>['ID', 'NAME', 'SALARY', 'DEPT', 'DOJ']</t>
         </is>
       </c>
-      <c r="F12" s="6" t="inlineStr">
+      <c r="F12" s="7" t="inlineStr">
         <is>
           <t>APROVADO</t>
         </is>
       </c>
       <c r="G12" s="1" t="n"/>
     </row>
-    <row r="13" ht="30" customHeight="1" s="14">
-      <c r="A13" s="4" t="n">
+    <row r="13">
+      <c r="A13" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Conteúdo das linhas (em ordem)</t>
+        </is>
+      </c>
+      <c r="C13" s="9" t="n">
+        <v>44799.63413583221</v>
+      </c>
+      <c r="D13" s="11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>MESMO CONTEÚDO DO SAS, NA ORDEM</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>APROVADO</t>
+        </is>
+      </c>
+      <c r="G13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
         <is>
           <t>Conteúdo das linhas</t>
         </is>
       </c>
-      <c r="C13" s="8" t="n">
-        <v>44796.6055871412</v>
-      </c>
-      <c r="D13" s="11" t="inlineStr">
+      <c r="C14" s="10" t="n">
+        <v>44799.63413577434</v>
+      </c>
+      <c r="D14" s="12" t="inlineStr">
         <is>
           <t>OK</t>
         </is>
       </c>
-      <c r="E13" s="11" t="inlineStr">
-        <is>
-          <t>MESMO CONTEÚDO DO SAS, NA ORDEM</t>
-        </is>
-      </c>
-      <c r="F13" s="7" t="inlineStr">
+      <c r="E14" s="12" t="inlineStr">
+        <is>
+          <t>MESMO CONTEÚDO</t>
+        </is>
+      </c>
+      <c r="F14" s="7" t="inlineStr">
         <is>
           <t>APROVADO</t>
         </is>
       </c>
-      <c r="G13" s="1" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>Conteúdo das linhas (em ordem)</t>
-        </is>
-      </c>
-      <c r="C14" s="9" t="n">
-        <v>44796.60558695602</v>
-      </c>
-      <c r="D14" s="12" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="E14" s="12" t="inlineStr">
-        <is>
-          <t>MESMO CONTEÚDO</t>
-        </is>
-      </c>
-      <c r="F14" s="6" t="inlineStr">
-        <is>
-          <t>APROVADO</t>
-        </is>
-      </c>
       <c r="G14" s="1" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="n">
+      <c r="A15" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B15" s="3" t="inlineStr">
         <is>
           <t>Tipo das Colunas</t>
         </is>
       </c>
-      <c r="C15" s="8" t="n">
-        <v>44796.6057184838</v>
-      </c>
-      <c r="D15" s="11" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="E15" s="11" t="inlineStr">
-        <is>
-          <t>Todos os campos equivalentes</t>
-        </is>
-      </c>
-      <c r="F15" s="7" t="inlineStr">
-        <is>
-          <t>APROVADO</t>
-        </is>
-      </c>
+      <c r="C15" s="9" t="n"/>
+      <c r="D15" s="11" t="n"/>
+      <c r="E15" s="11" t="n"/>
+      <c r="F15" s="8" t="n"/>
       <c r="G15" s="1" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" s="4" t="inlineStr">
         <is>
           <t>Teste do formato de datas</t>
         </is>
       </c>
-      <c r="C16" s="9" t="n">
-        <v>44796.64952684756</v>
-      </c>
-      <c r="D16" s="12" t="inlineStr">
-        <is>
-          <t>YYMMDD10</t>
-        </is>
-      </c>
-      <c r="E16" s="12" t="inlineStr">
-        <is>
-          <t>%Y-%m-%d</t>
-        </is>
-      </c>
-      <c r="F16" s="6" t="inlineStr">
-        <is>
-          <t>APROVADO</t>
-        </is>
-      </c>
+      <c r="C16" s="10" t="n"/>
+      <c r="D16" s="12" t="n"/>
+      <c r="E16" s="12" t="n"/>
+      <c r="F16" s="7" t="n"/>
       <c r="G16" s="1" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n">
+      <c r="A17" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B17" s="2" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>Performance</t>
         </is>
       </c>
-      <c r="C17" s="8" t="n"/>
+      <c r="C17" s="9" t="n"/>
       <c r="D17" s="11" t="n"/>
       <c r="E17" s="11" t="n"/>
-      <c r="F17" s="7" t="n"/>
+      <c r="F17" s="8" t="n"/>
       <c r="G17" s="1" t="n"/>
     </row>
-    <row r="18" ht="30" customHeight="1" s="14">
-      <c r="A18" s="5" t="n">
+    <row r="18">
+      <c r="A18" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B18" s="4" t="inlineStr">
         <is>
           <t>Periodo do relatório</t>
         </is>
       </c>
-      <c r="C18" s="9" t="n">
-        <v>44796.64952684756</v>
-      </c>
-      <c r="D18" s="12" t="inlineStr">
-        <is>
-          <t>[    16/08/1998-    13/09/2014]</t>
-        </is>
-      </c>
-      <c r="E18" s="12" t="inlineStr">
-        <is>
-          <t>[    16/08/1998-    13/09/2014]</t>
-        </is>
-      </c>
-      <c r="F18" s="6" t="inlineStr">
-        <is>
-          <t>APROVADO</t>
-        </is>
-      </c>
+      <c r="C18" s="10" t="n"/>
+      <c r="D18" s="12" t="n"/>
+      <c r="E18" s="12" t="n"/>
+      <c r="F18" s="7" t="n"/>
       <c r="G18" s="1" t="n"/>
     </row>
     <row r="19">

</xml_diff>